<commit_message>
Added graphbased image segmentation code
</commit_message>
<xml_diff>
--- a/Wishlist/Wishlist.xlsx
+++ b/Wishlist/Wishlist.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>Item</t>
   </si>
@@ -43,6 +43,9 @@
   </si>
   <si>
     <t>Hardware to make a pole for GPS</t>
+  </si>
+  <si>
+    <t>Total</t>
   </si>
 </sst>
 </file>
@@ -397,16 +400,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B8"/>
+  <dimension ref="A1:B10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="34.85546875" customWidth="1"/>
-    <col min="2" max="2" width="9.140625" style="3"/>
+    <col min="2" max="2" width="10.5703125" style="3" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
@@ -471,6 +474,15 @@
       </c>
       <c r="B8" s="3">
         <v>150</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2">
+      <c r="A10" t="s">
+        <v>9</v>
+      </c>
+      <c r="B10" s="3">
+        <f>SUM(B2:B8)</f>
+        <v>1630</v>
       </c>
     </row>
   </sheetData>

</xml_diff>